<commit_message>
Atualização dados de 20/07
</commit_message>
<xml_diff>
--- a/Sergipe/data_general/historico_sergipe.xlsx
+++ b/Sergipe/data_general/historico_sergipe.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adolfoguimaraes/Dev/DataViz/covid19-br/Vacinacao/Sergipe/data_general/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFE8BDE1-1B39-C043-807D-1743177EB4F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8F5641E-49E5-5A49-8DCC-3D87A4635FDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="20000" windowHeight="14860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -477,10 +477,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G123"/>
+  <dimension ref="A1:G124"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A106" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D123" sqref="D123"/>
+      <selection activeCell="B124" sqref="B124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3321,6 +3321,29 @@
         <v>38700</v>
       </c>
     </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A124" s="2">
+        <v>44397</v>
+      </c>
+      <c r="B124">
+        <v>931761</v>
+      </c>
+      <c r="C124">
+        <v>943038</v>
+      </c>
+      <c r="D124">
+        <v>429995</v>
+      </c>
+      <c r="E124">
+        <v>284674</v>
+      </c>
+      <c r="F124" s="5">
+        <v>38700</v>
+      </c>
+      <c r="G124" s="5">
+        <v>38700</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Atualização até o dia 13/09
</commit_message>
<xml_diff>
--- a/Sergipe/data_general/historico_sergipe.xlsx
+++ b/Sergipe/data_general/historico_sergipe.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adolfoguimaraes/Dev/DataViz/covid19-br/Vacinacao/Sergipe/data_general/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DBA6ABC-98A7-3C46-AB05-33CFDE511130}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5892AE9-CFEB-F24C-85F7-B104D0C25B24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38400" yWindow="500" windowWidth="27320" windowHeight="14860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -477,10 +477,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G156"/>
+  <dimension ref="A1:G172"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A136" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="G156" sqref="G156"/>
+    <sheetView tabSelected="1" topLeftCell="A154" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D168" sqref="D168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4080,6 +4080,374 @@
         <v>39485</v>
       </c>
     </row>
+    <row r="157" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A157" s="2">
+        <v>44433</v>
+      </c>
+      <c r="B157">
+        <v>1482236</v>
+      </c>
+      <c r="C157">
+        <v>1335021</v>
+      </c>
+      <c r="D157">
+        <v>667299</v>
+      </c>
+      <c r="E157">
+        <v>457579</v>
+      </c>
+      <c r="F157">
+        <v>39750</v>
+      </c>
+      <c r="G157">
+        <v>39485</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A158" s="2">
+        <v>44434</v>
+      </c>
+      <c r="B158">
+        <v>1482236</v>
+      </c>
+      <c r="C158">
+        <v>1349019</v>
+      </c>
+      <c r="D158">
+        <v>667299</v>
+      </c>
+      <c r="E158">
+        <v>466482</v>
+      </c>
+      <c r="F158">
+        <v>39750</v>
+      </c>
+      <c r="G158">
+        <v>39485</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A159" s="2">
+        <v>44435</v>
+      </c>
+      <c r="B159">
+        <v>1482236</v>
+      </c>
+      <c r="C159">
+        <v>1357601</v>
+      </c>
+      <c r="D159">
+        <v>667299</v>
+      </c>
+      <c r="E159">
+        <v>475016</v>
+      </c>
+      <c r="F159">
+        <v>39750</v>
+      </c>
+      <c r="G159">
+        <v>39485</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A160" s="2">
+        <v>44436</v>
+      </c>
+      <c r="B160">
+        <v>1482236</v>
+      </c>
+      <c r="C160">
+        <v>1400631</v>
+      </c>
+      <c r="D160">
+        <v>667299</v>
+      </c>
+      <c r="E160">
+        <v>478997</v>
+      </c>
+      <c r="F160">
+        <v>39750</v>
+      </c>
+      <c r="G160">
+        <v>39942</v>
+      </c>
+    </row>
+    <row r="161" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A161" s="2">
+        <v>44438</v>
+      </c>
+      <c r="B161">
+        <v>1482236</v>
+      </c>
+      <c r="C161">
+        <v>1417132</v>
+      </c>
+      <c r="D161">
+        <v>667299</v>
+      </c>
+      <c r="E161">
+        <v>490232</v>
+      </c>
+      <c r="F161">
+        <v>39750</v>
+      </c>
+      <c r="G161">
+        <v>39952</v>
+      </c>
+    </row>
+    <row r="162" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A162" s="2">
+        <v>44439</v>
+      </c>
+      <c r="B162">
+        <v>1505856</v>
+      </c>
+      <c r="C162">
+        <v>1420471</v>
+      </c>
+      <c r="D162">
+        <v>800786</v>
+      </c>
+      <c r="E162">
+        <v>497561</v>
+      </c>
+      <c r="F162">
+        <v>39750</v>
+      </c>
+      <c r="G162">
+        <v>39952</v>
+      </c>
+    </row>
+    <row r="163" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A163" s="2">
+        <v>44440</v>
+      </c>
+      <c r="B163">
+        <v>1505856</v>
+      </c>
+      <c r="C163">
+        <v>1426524</v>
+      </c>
+      <c r="D163">
+        <v>800786</v>
+      </c>
+      <c r="E163">
+        <v>509292</v>
+      </c>
+      <c r="F163">
+        <v>39750</v>
+      </c>
+      <c r="G163">
+        <v>39952</v>
+      </c>
+    </row>
+    <row r="164" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A164" s="2">
+        <v>44441</v>
+      </c>
+      <c r="B164">
+        <v>1505856</v>
+      </c>
+      <c r="C164">
+        <v>1430500</v>
+      </c>
+      <c r="D164">
+        <v>800786</v>
+      </c>
+      <c r="E164">
+        <v>526185</v>
+      </c>
+      <c r="F164">
+        <v>39750</v>
+      </c>
+      <c r="G164">
+        <v>39952</v>
+      </c>
+    </row>
+    <row r="165" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A165" s="2">
+        <v>44442</v>
+      </c>
+      <c r="B165">
+        <v>1505856</v>
+      </c>
+      <c r="C165">
+        <v>1433995</v>
+      </c>
+      <c r="D165">
+        <v>800786</v>
+      </c>
+      <c r="E165">
+        <v>535772</v>
+      </c>
+      <c r="F165">
+        <v>39750</v>
+      </c>
+      <c r="G165">
+        <v>39952</v>
+      </c>
+    </row>
+    <row r="166" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A166" s="2">
+        <v>44443</v>
+      </c>
+      <c r="B166">
+        <v>1505856</v>
+      </c>
+      <c r="C166">
+        <v>1434678</v>
+      </c>
+      <c r="D166">
+        <v>800786</v>
+      </c>
+      <c r="E166">
+        <v>538935</v>
+      </c>
+      <c r="F166">
+        <v>39750</v>
+      </c>
+      <c r="G166">
+        <v>39952</v>
+      </c>
+    </row>
+    <row r="167" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A167" s="2">
+        <v>44445</v>
+      </c>
+      <c r="B167">
+        <v>1505856</v>
+      </c>
+      <c r="C167">
+        <v>1435077</v>
+      </c>
+      <c r="D167">
+        <v>800786</v>
+      </c>
+      <c r="E167">
+        <v>552857</v>
+      </c>
+      <c r="F167">
+        <v>39750</v>
+      </c>
+      <c r="G167">
+        <v>39952</v>
+      </c>
+    </row>
+    <row r="168" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A168" s="2">
+        <v>44447</v>
+      </c>
+      <c r="B168">
+        <v>1505856</v>
+      </c>
+      <c r="C168">
+        <v>1436753</v>
+      </c>
+      <c r="D168">
+        <v>800786</v>
+      </c>
+      <c r="E168">
+        <v>565854</v>
+      </c>
+      <c r="F168">
+        <v>39750</v>
+      </c>
+      <c r="G168">
+        <v>39952</v>
+      </c>
+    </row>
+    <row r="169" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A169" s="2">
+        <v>44448</v>
+      </c>
+      <c r="B169">
+        <v>1527766</v>
+      </c>
+      <c r="C169">
+        <v>1443028</v>
+      </c>
+      <c r="D169">
+        <v>914366</v>
+      </c>
+      <c r="E169">
+        <v>588034</v>
+      </c>
+      <c r="F169">
+        <v>39750</v>
+      </c>
+      <c r="G169">
+        <v>39952</v>
+      </c>
+    </row>
+    <row r="170" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A170" s="2">
+        <v>44449</v>
+      </c>
+      <c r="B170">
+        <v>1527766</v>
+      </c>
+      <c r="C170">
+        <v>1451814</v>
+      </c>
+      <c r="D170">
+        <v>914366</v>
+      </c>
+      <c r="E170">
+        <v>602888</v>
+      </c>
+      <c r="F170">
+        <v>39750</v>
+      </c>
+      <c r="G170">
+        <v>39952</v>
+      </c>
+    </row>
+    <row r="171" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A171" s="2">
+        <v>44450</v>
+      </c>
+      <c r="B171">
+        <v>1527766</v>
+      </c>
+      <c r="C171">
+        <v>1453771</v>
+      </c>
+      <c r="D171">
+        <v>914366</v>
+      </c>
+      <c r="E171">
+        <v>606539</v>
+      </c>
+      <c r="F171">
+        <v>39750</v>
+      </c>
+      <c r="G171">
+        <v>39952</v>
+      </c>
+    </row>
+    <row r="172" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A172" s="2">
+        <v>44452</v>
+      </c>
+      <c r="B172">
+        <v>1527766</v>
+      </c>
+      <c r="C172">
+        <v>1462728</v>
+      </c>
+      <c r="D172">
+        <v>914366</v>
+      </c>
+      <c r="E172">
+        <v>634665</v>
+      </c>
+      <c r="F172">
+        <v>39750</v>
+      </c>
+      <c r="G172">
+        <v>39952</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Atualização dados 15 e 16/10
</commit_message>
<xml_diff>
--- a/Sergipe/data_general/historico_sergipe.xlsx
+++ b/Sergipe/data_general/historico_sergipe.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10912"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adolfoguimaraes/Dev/DataViz/covid19-br/Vacinacao/Sergipe/data_general/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A64D90A-4AC8-B74C-9E38-EDAE3BE1F652}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FC5736D-FCE5-9A4A-A7E6-EB12EC9FEC3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38400" yWindow="500" windowWidth="27320" windowHeight="14860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -477,10 +477,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G173"/>
+  <dimension ref="A1:G175"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A154" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E168" sqref="E168"/>
+    <sheetView tabSelected="1" topLeftCell="A156" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D175" sqref="D175"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4471,6 +4471,52 @@
         <v>40023</v>
       </c>
     </row>
+    <row r="174" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A174" s="2">
+        <v>44454</v>
+      </c>
+      <c r="B174">
+        <v>1602737</v>
+      </c>
+      <c r="C174">
+        <v>1480519</v>
+      </c>
+      <c r="D174">
+        <v>921386</v>
+      </c>
+      <c r="E174">
+        <v>700142</v>
+      </c>
+      <c r="F174">
+        <v>39750</v>
+      </c>
+      <c r="G174">
+        <v>40023</v>
+      </c>
+    </row>
+    <row r="175" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A175" s="2">
+        <v>44455</v>
+      </c>
+      <c r="B175">
+        <v>1602737</v>
+      </c>
+      <c r="C175">
+        <v>1489443</v>
+      </c>
+      <c r="D175">
+        <v>921386</v>
+      </c>
+      <c r="E175">
+        <v>708689</v>
+      </c>
+      <c r="F175">
+        <v>39750</v>
+      </c>
+      <c r="G175">
+        <v>40023</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>